<commit_message>
Vin(max) modified as 250V.
</commit_message>
<xml_diff>
--- a/Buck_Converter/Buck_Converter_Calculations.xlsx
+++ b/Buck_Converter/Buck_Converter_Calculations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\Education\EE\EE4.1\EE463\TermProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\EE463-Term-Project\Buck_Converter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DFEA2D-8508-40C6-8689-632A08CC4D4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4395B38C-5D75-41B1-908E-DBBC538A3BC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43F1BF6C-91A1-474F-8104-A1424F633C63}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Vin</t>
   </si>
@@ -52,21 +52,6 @@
   </si>
   <si>
     <t>L</t>
-  </si>
-  <si>
-    <t>Toplam</t>
-  </si>
-  <si>
-    <t>Ortalama</t>
-  </si>
-  <si>
-    <t>Değişen Toplam</t>
-  </si>
-  <si>
-    <t>Say</t>
-  </si>
-  <si>
-    <t>Sütun3</t>
   </si>
   <si>
     <t>∆Vout</t>
@@ -691,7 +676,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCAA62E4-00D6-467F-AF21-D184D39D3DB5}">
   <dimension ref="A2:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -705,7 +692,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>100</v>
+        <v>250</v>
       </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
@@ -727,7 +714,7 @@
       </c>
       <c r="F3">
         <f>B8/B7</f>
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
@@ -749,7 +736,7 @@
       </c>
       <c r="F4">
         <f>((B2-B3-B4)*(B5+B4))/((B2-B3+B5)*B6*F3*B7)</f>
-        <v>3.8722729091636653E-3</v>
+        <v>5.963248801916933E-3</v>
       </c>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
@@ -764,14 +751,14 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>0.26</v>
+        <v>0.7</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F5">
         <f>(B8/(8*B6))*(1/(B9-(B8*B11)-(B12*B10/F4)))</f>
-        <v>6.2149019095173902E-6</v>
+        <v>4.0957909231832734E-6</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
@@ -789,11 +776,11 @@
         <v>10000</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="F6">
         <f>1/(2*PI()*SQRT(F4*F5))</f>
-        <v>1025.935395337506</v>
+        <v>1018.379802168795</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
@@ -811,11 +798,11 @@
         <v>2</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F7">
         <f>((1-(B4/B2))*B14*B4)/(B6*B2*(B16-((1-(B4/B2))*B14*B15)))</f>
-        <v>1.4502843829233195E-6</v>
+        <v>7.0656225874048757E-7</v>
       </c>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
@@ -830,10 +817,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
@@ -845,7 +832,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>1.84</v>
@@ -860,10 +847,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B10">
-        <v>265</v>
+        <v>250</v>
       </c>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
@@ -875,10 +862,10 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -890,7 +877,7 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>1.0000000000000001E-5</v>
@@ -905,7 +892,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B13">
         <v>30</v>
@@ -920,7 +907,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>2.2000000000000002</v>
@@ -935,7 +922,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>0.5</v>
@@ -950,7 +937,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>30</v>

</xml_diff>